<commit_message>
Updated Penman and added Penman openwater example
</commit_message>
<xml_diff>
--- a/examples/data/example_0/df_Guo_2016.xlsx
+++ b/examples/data/example_0/df_Guo_2016.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\pyet\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\pyet\examples\data\example_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E31F2C-3B9A-4BA3-AAE1-8EEC902B559B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98C2F3F-794D-4912-8C87-897D0B9027F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:V1281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +952,7 @@
         <v>6.1189809163939204</v>
       </c>
       <c r="S8">
-        <v>7.9645390362859896</v>
+        <v>7.9444390362859902</v>
       </c>
       <c r="T8">
         <v>6.3031531364330702</v>

</xml_diff>